<commit_message>
Arrays and Basic programs on 29.03.2025
</commit_message>
<xml_diff>
--- a/javaPrograms.xlsx
+++ b/javaPrograms.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amisharm49\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\newEclipseWorkspace\JavaPrograms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18E56D7-24D1-43BF-BD12-4561F8017199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="4" xr2:uid="{9ED84348-7B0E-4DA5-9846-BD597D73BDB4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="RS_interview" sheetId="1" r:id="rId1"/>
     <sheet name="Pattern" sheetId="2" r:id="rId2"/>
-    <sheet name="Arrays" sheetId="3" r:id="rId3"/>
-    <sheet name="Strings" sheetId="4" r:id="rId4"/>
-    <sheet name="Basics" sheetId="5" r:id="rId5"/>
+    <sheet name="Basics" sheetId="5" r:id="rId3"/>
+    <sheet name="Arrays" sheetId="9" r:id="rId4"/>
+    <sheet name="Strings" sheetId="4" r:id="rId5"/>
     <sheet name="Streams" sheetId="6" r:id="rId6"/>
     <sheet name="LinkedinCodes" sheetId="7" r:id="rId7"/>
     <sheet name="Interview" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Basics!$A$1:$E$22</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="153">
   <si>
     <t>Create a method which accepts Array and return sum of all the elements of arrays</t>
   </si>
@@ -438,12 +440,331 @@
 reverse = reverse * 10 + n;
 num = num/10;</t>
   </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <r>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>((</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A3E3E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'a'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &amp;&amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A3E3E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'z'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) || (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A3E3E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'A'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &amp;&amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A3E3E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Z'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>for(int i=0; i&lt;exponent ; i++) {
+   result = result * base;</t>
+  </si>
+  <si>
+    <t>for(int i=num; i&gt;0; i--) {
+   fact = fact * i;</t>
+  </si>
+  <si>
+    <t>153 = cube(1) + cube(5) + cube(3)
+while(num!=0) {
+   int n = num % 10;
+   result = result + Math.pow(n, 3);
+   num = num / 10;</t>
+  </si>
+  <si>
+    <t>Print elements of an array</t>
+  </si>
+  <si>
+    <t>Copy one array to another.</t>
+  </si>
+  <si>
+    <t>Print elements of an array in reverse order</t>
+  </si>
+  <si>
+    <t>Print elements in array at even and odd positions</t>
+  </si>
+  <si>
+    <t>Sum of all elements of an array</t>
+  </si>
+  <si>
+    <r>
+      <t>sum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A3E3E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>sum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A3E3E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF6A3E3E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>];</t>
+    </r>
+  </si>
+  <si>
+    <t>Sort elements of an array in ascending order</t>
+  </si>
+  <si>
+    <t>Sort elements of an array in descending order</t>
+  </si>
+  <si>
+    <t>if(a[i] &lt; a[j]) {</t>
+  </si>
+  <si>
+    <t>Print largest and second largest element in an array</t>
+  </si>
+  <si>
+    <t>Print Smallest and second smallest element in an array</t>
+  </si>
+  <si>
+    <t>Sort the array in ascending order
+Largest element = a[a.length-1]
+Second Largest element = a[a.length-2]</t>
+  </si>
+  <si>
+    <t>Smallest element = a[0]
+Second smallest element = a[1]</t>
+  </si>
+  <si>
+    <t>Print duplicate elements in an array</t>
+  </si>
+  <si>
+    <t>Left rotate</t>
+  </si>
+  <si>
+    <t>Right rotate</t>
+  </si>
+  <si>
+    <t>Program to find missing number in an integer array</t>
+  </si>
+  <si>
+    <t>Program to find frequency of each element in an array</t>
+  </si>
+  <si>
+    <t>Program to join 2 arrays</t>
+  </si>
+  <si>
+    <t>Shift all zeros to the right side</t>
+  </si>
+  <si>
+    <t>Shift all zeros to the left side</t>
+  </si>
+  <si>
+    <t>for(int i=0; i&lt;a.length; i++) {
+   for(int j=i+1; j&lt;a.length; j++) {
+    if(a[i] &gt; a[j]) {
+     temp = a[i];
+     a[i] = a[j];
+     a[j] = temp;}  }
+  }</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,6 +789,25 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A3E3E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -497,7 +837,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -505,11 +845,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -529,8 +884,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,25 +1235,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADFA35F6-1128-434C-8E07-DDFB3FD13038}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="92.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="92.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -890,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -898,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -906,7 +1277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -914,7 +1285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -922,7 +1293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -930,7 +1301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -938,7 +1309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -946,7 +1317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -954,7 +1325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -962,7 +1333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -970,7 +1341,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -981,7 +1352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -989,7 +1360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -997,7 +1368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1005,7 +1376,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1013,7 +1384,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1021,7 +1392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1029,7 +1400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1043,164 +1414,164 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C6952AD-4932-4E1F-8B55-D3A6BB381EE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="2" t="s">
         <v>45</v>
       </c>
@@ -1211,305 +1582,700 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0CE4EA-DC67-444A-97CE-7AD4C17C0CCA}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="80.625" customWidth="1"/>
+    <col min="4" max="4" width="48.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="42.75">
+      <c r="A12" s="11">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.5">
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="42.75">
+      <c r="A17" s="9">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="9">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.5">
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.5">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.5">
+      <c r="A21" s="9">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="71.25">
+      <c r="A22" s="9">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E22"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5656BE-2701-40DC-A103-AFE84694C26D}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="72.125" customWidth="1"/>
+    <col min="4" max="4" width="53.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="99.75">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="42.75">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.5">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="9">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="9">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED23A3B7-74D0-4A5A-BC8E-7605A9A3FF55}">
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="80.5703125" customWidth="1"/>
-    <col min="4" max="4" width="48.42578125" customWidth="1"/>
+    <col min="2" max="2" width="72.125" customWidth="1"/>
+    <col min="4" max="4" width="53.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="14" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" t="s">
-        <v>49</v>
-      </c>
+      <c r="E1" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1517,48 +2283,48 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9018AD35-4702-4C04-8698-AA1917B29CEF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709951FB-1CF9-4CCE-9E59-2C7E83238BBB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F361AD86-66BC-4C66-816F-F2FE5737FB5E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="8" t="s">
         <v>61</v>
       </c>
@@ -1572,7 +2338,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1583,7 +2349,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1600,7 +2366,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1611,7 +2377,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1622,7 +2388,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1633,7 +2399,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1644,7 +2410,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="71.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1658,7 +2424,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1669,7 +2435,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1680,7 +2446,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1691,7 +2457,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1702,7 +2468,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1710,7 +2476,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1718,7 +2484,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1726,7 +2492,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1737,7 +2503,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1745,7 +2511,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1756,7 +2522,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1764,7 +2530,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1775,7 +2541,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1783,7 +2549,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1794,7 +2560,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1802,7 +2568,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1810,7 +2576,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1818,7 +2584,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="28.5">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1826,7 +2592,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="28.5">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1834,7 +2600,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="28.5">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1842,7 +2608,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="28.5">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1850,7 +2616,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="28.5">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1858,7 +2624,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1866,7 +2632,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1874,7 +2640,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1882,7 +2648,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1890,7 +2656,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1898,7 +2664,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1906,7 +2672,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1914,7 +2680,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1922,7 +2688,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1930,7 +2696,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1938,7 +2704,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1946,7 +2712,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1954,7 +2720,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="28.5">
       <c r="A43">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
new commit on 24.07.2025
</commit_message>
<xml_diff>
--- a/javaPrograms.xlsx
+++ b/javaPrograms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amisharm49\eclipse-workspace\JavaPrograms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643A7B4C-F770-48E6-BFDF-9109629C4136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A365F14-B9DE-4344-9410-77B23305B544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RS_interview" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="232">
   <si>
     <t>Create a method which accepts Array and return sum of all the elements of arrays</t>
   </si>
@@ -744,12 +744,6 @@
      a[i] = a[j];
      a[j] = temp;}  }
   }</t>
-  </si>
-  <si>
-    <t>Method 1 : Sort the array in ascending order</t>
-  </si>
-  <si>
-    <t>Method 1 : Sort the array in descending order</t>
   </si>
   <si>
     <t>Remove duplicate elements from an array</t>
@@ -1562,6 +1556,13 @@
   </si>
   <si>
     <t>Create a new Set and add array elements to it. Create a new array with size of set and add set elements to the new array.</t>
+  </si>
+  <si>
+    <t>Join 2 arrays using 2 loops.</t>
+  </si>
+  <si>
+    <t>Sorted array (with Temp or without temp array)
+Unsorted array  ( sorting, using Maps, Using Sets)</t>
   </si>
 </sst>
 </file>
@@ -1693,7 +1694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1734,17 +1735,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2090,7 +2083,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,8 +2447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2646,7 +2639,7 @@
         <v>49</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>124</v>
@@ -2827,10 +2820,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2856,7 +2850,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2867,13 +2861,13 @@
         <v>47</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2888,7 +2882,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2903,7 +2897,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2918,7 +2912,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -2935,7 +2929,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2952,7 +2946,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2969,7 +2963,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2986,7 +2980,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3003,7 +2997,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3014,7 +3008,7 @@
         <v>49</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>124</v>
@@ -3033,7 +3027,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -3044,9 +3038,11 @@
         <v>49</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -3057,9 +3053,11 @@
         <v>49</v>
       </c>
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -3074,7 +3072,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -3084,10 +3082,14 @@
       <c r="C16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -3097,12 +3099,12 @@
       <c r="C17" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -3112,36 +3114,45 @@
       <c r="C18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="D19" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E19" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
+  <autoFilter ref="A1:E19" xr:uid="{00000000-0001-0000-0300-000000000000}">
+    <filterColumn colId="4">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3167,12 +3178,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>47</v>
@@ -3182,12 +3193,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>47</v>
@@ -3197,18 +3208,18 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>124</v>
@@ -3219,24 +3230,24 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>124</v>
@@ -3247,92 +3258,92 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>124</v>
@@ -3343,7 +3354,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -3354,11 +3365,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="17" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -3367,18 +3378,18 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>49</v>
@@ -3393,58 +3404,58 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>124</v>
@@ -3455,31 +3466,35 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>124</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E22" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <autoFilter ref="A1:E22" xr:uid="{00000000-0001-0000-0400-000000000000}">
+    <filterColumn colId="4">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3488,8 +3503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3520,13 +3535,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>124</v>
@@ -3537,13 +3552,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>124</v>
@@ -3554,13 +3569,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>124</v>
@@ -3571,13 +3586,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>124</v>
@@ -3588,13 +3603,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>124</v>
@@ -3605,13 +3620,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>124</v>
@@ -3622,13 +3637,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>124</v>
@@ -3639,13 +3654,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>124</v>
@@ -3656,13 +3671,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>124</v>
@@ -3673,13 +3688,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>124</v>
@@ -3690,13 +3705,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>124</v>
@@ -3707,13 +3722,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>124</v>
@@ -3724,13 +3739,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>124</v>
@@ -3741,24 +3756,24 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -3775,7 +3790,7 @@
   <dimension ref="B2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3785,12 +3800,12 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3802,31 +3817,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="18"/>
     <col min="4" max="4" width="86.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="18" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3834,10 +3848,10 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D2" s="5"/>
@@ -3849,10 +3863,10 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -3866,10 +3880,10 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D4" s="5"/>
@@ -3881,10 +3895,10 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D5" s="5"/>
@@ -3896,10 +3910,10 @@
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D6" s="5"/>
@@ -3911,10 +3925,10 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D7" s="5"/>
@@ -3926,10 +3940,10 @@
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -3943,10 +3957,10 @@
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D9" s="5"/>
@@ -3958,10 +3972,10 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="5"/>
@@ -3973,10 +3987,10 @@
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="5"/>
@@ -3988,10 +4002,10 @@
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="5"/>
@@ -4003,14 +4017,14 @@
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>124</v>
@@ -4020,10 +4034,10 @@
       <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D14" s="5"/>
@@ -4033,10 +4047,10 @@
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="5"/>
@@ -4046,10 +4060,10 @@
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D16" s="5"/>
@@ -4061,10 +4075,10 @@
       <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="5"/>
@@ -4074,14 +4088,14 @@
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>124</v>
@@ -4091,14 +4105,14 @@
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>124</v>
@@ -4108,10 +4122,10 @@
       <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D20" s="5"/>
@@ -4123,10 +4137,10 @@
       <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="5"/>
@@ -4136,10 +4150,10 @@
       <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D22" s="5"/>
@@ -4151,10 +4165,10 @@
       <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D23" s="5"/>
@@ -4166,14 +4180,14 @@
       <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>124</v>
@@ -4183,10 +4197,10 @@
       <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="5"/>
@@ -4198,10 +4212,10 @@
       <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D26" s="5"/>
@@ -4211,10 +4225,10 @@
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="5"/>
@@ -4226,10 +4240,10 @@
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D28" s="5"/>
@@ -4241,10 +4255,10 @@
       <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D29" s="5"/>
@@ -4254,10 +4268,10 @@
       <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D30" s="5"/>
@@ -4267,10 +4281,10 @@
       <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="5" t="s">
         <v>49</v>
       </c>
       <c r="D31" s="5"/>
@@ -4283,11 +4297,11 @@
       <c r="B32" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>124</v>
@@ -4300,11 +4314,11 @@
       <c r="B33" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>124</v>
@@ -4317,7 +4331,7 @@
       <c r="B34" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D34" s="5"/>
@@ -4332,13 +4346,15 @@
       <c r="B35" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="E35" s="5"/>
+        <v>229</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
@@ -4347,11 +4363,11 @@
       <c r="B36" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>124</v>
@@ -4364,7 +4380,7 @@
       <c r="B37" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D37" s="5"/>
@@ -4379,11 +4395,11 @@
       <c r="B38" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>124</v>
@@ -4396,7 +4412,7 @@
       <c r="B39" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D39" s="5"/>
@@ -4411,11 +4427,11 @@
       <c r="B40" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>124</v>
@@ -4428,11 +4444,11 @@
       <c r="B41" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>124</v>
@@ -4445,7 +4461,7 @@
       <c r="B42" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="22" t="s">
+      <c r="C42" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D42" s="5"/>
@@ -4457,10 +4473,10 @@
       <c r="A43" s="5">
         <v>42</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D43" s="5"/>

</xml_diff>